<commit_message>
Actualização do contacto do David João
</commit_message>
<xml_diff>
--- a/Contactos.xlsx
+++ b/Contactos.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="105" windowWidth="15120" windowHeight="8010"/>
@@ -72,8 +72,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -140,6 +140,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -218,6 +223,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -252,6 +258,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -427,21 +434,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.28515625" customWidth="1"/>
     <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="30.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -452,7 +459,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
@@ -463,16 +470,18 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="2"/>
+      <c r="B3" s="2">
+        <v>919659339</v>
+      </c>
       <c r="C3" s="3" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
@@ -483,7 +492,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
@@ -494,7 +503,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>7</v>
       </c>
@@ -508,7 +517,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>8</v>
       </c>
@@ -519,7 +528,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>9</v>
       </c>
@@ -544,12 +553,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
@@ -557,12 +566,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>

</xml_diff>